<commit_message>
Updated the xlsx files with mec prod data.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/biometric_attribute.xlsx
+++ b/mosip_master/xlsx/biometric_attribute.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\Mosip Codebase\Chithara27-fork\MEC-PROD-Mosip-data excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E1951A-F770-4F32-B7B6-F482E1E9CF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>lang_code</t>
   </si>
@@ -59,9 +60,6 @@
     <t>FNR</t>
   </si>
   <si>
-    <t>TRUE</t>
-  </si>
-  <si>
     <t>RH</t>
   </si>
   <si>
@@ -101,76 +99,34 @@
     <t>Print of Right Iris</t>
   </si>
   <si>
-    <t>fra</t>
-  </si>
-  <si>
-    <t>Les pouces</t>
-  </si>
-  <si>
-    <t>Empreinte des pouces gauche et droit</t>
-  </si>
-  <si>
-    <t>Dalle droite</t>
-  </si>
-  <si>
-    <t>Impression de la dalle droite</t>
-  </si>
-  <si>
-    <t>Dalle gauche</t>
-  </si>
-  <si>
-    <t>Impression de la dalle gauche</t>
-  </si>
-  <si>
-    <t>Iris gauche</t>
-  </si>
-  <si>
-    <t>Gravure de Iris Gauche</t>
-  </si>
-  <si>
-    <t>Iris droit</t>
-  </si>
-  <si>
-    <t>Empreinte de l'iris droit</t>
-  </si>
-  <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>الإبهام</t>
-  </si>
-  <si>
-    <t>اللوح الأيمن</t>
-  </si>
-  <si>
-    <t>اللوح الأيسر</t>
-  </si>
-  <si>
-    <t>اليسار ايريس</t>
-  </si>
-  <si>
-    <t>حق ايريس</t>
-  </si>
-  <si>
-    <t>طباعة الإبهام الأيمن والأيسر</t>
-  </si>
-  <si>
-    <t>طباعة اللوح الأيمن</t>
-  </si>
-  <si>
-    <t>طباعة اللوح الأيسر</t>
-  </si>
-  <si>
-    <t>طباعة القزحية اليمنى</t>
-  </si>
-  <si>
-    <t>طباعة القزحية اليسرى</t>
+    <t>cr_by</t>
+  </si>
+  <si>
+    <t>cr_dtimes</t>
+  </si>
+  <si>
+    <t>upd_by</t>
+  </si>
+  <si>
+    <t>upd_dtimes</t>
+  </si>
+  <si>
+    <t>is_deleted</t>
+  </si>
+  <si>
+    <t>del_dtimes</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>rediet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,10 +136,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <charset val="1"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -231,6 +186,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,63 +467,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1"/>
+    <col min="1" max="1" width="25.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="22.36328125" customWidth="1"/>
+    <col min="4" max="4" width="35.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="6">
+        <v>44776.354283958332</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -575,18 +565,30 @@
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6">
+        <v>44776.354283958332</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>15</v>
@@ -595,18 +597,30 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="6">
+        <v>44776.354283958332</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>18</v>
@@ -618,15 +632,27 @@
         <v>20</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6">
+        <v>44776.354283958332</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>22</v>
@@ -635,214 +661,41 @@
         <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="H6" s="6">
+        <v>44776.354283958332</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>